<commit_message>
chore: add all feature documentation
</commit_message>
<xml_diff>
--- a/static/file/schools_import.xlsx
+++ b/static/file/schools_import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="122">
   <si>
     <t xml:space="preserve">Data Umum Sekolah</t>
   </si>
@@ -33,7 +33,7 @@
     <t xml:space="preserve">Nama Sekolah</t>
   </si>
   <si>
-    <t xml:space="preserve">SD Negeri 01 Pagi</t>
+    <t xml:space="preserve">nama sekolah</t>
   </si>
   <si>
     <t xml:space="preserve">Nomor Pokok Sekolah Nasional</t>
@@ -48,7 +48,7 @@
     <t xml:space="preserve">Alamat</t>
   </si>
   <si>
-    <t xml:space="preserve">Jalan Raya no 101 RT 003/004</t>
+    <t xml:space="preserve">alamat </t>
   </si>
   <si>
     <t xml:space="preserve">Email Sekolah (email resmi utk kontak)</t>
@@ -60,21 +60,15 @@
     <t xml:space="preserve">No Telpon Sekolah</t>
   </si>
   <si>
-    <t xml:space="preserve">081212341234</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nama Kepsek / Penanggungjawab Umum</t>
   </si>
   <si>
-    <t xml:space="preserve">Albert Einstein</t>
+    <t xml:space="preserve">kepsek</t>
   </si>
   <si>
     <t xml:space="preserve">NIK Kepsek</t>
   </si>
   <si>
-    <t xml:space="preserve">1234567812345678</t>
-  </si>
-  <si>
     <t xml:space="preserve">Email Kepsek</t>
   </si>
   <si>
@@ -84,21 +78,15 @@
     <t xml:space="preserve">No Telpon Kepsek (WA)</t>
   </si>
   <si>
-    <t xml:space="preserve">081343214321</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nama Admin (bila beda dgn Kepsek)</t>
   </si>
   <si>
-    <t xml:space="preserve">John Doe</t>
+    <t xml:space="preserve">admin</t>
   </si>
   <si>
     <t xml:space="preserve">NIK Admin</t>
   </si>
   <si>
-    <t xml:space="preserve">8765432187654321</t>
-  </si>
-  <si>
     <t xml:space="preserve">Email Admin</t>
   </si>
   <si>
@@ -397,18 +385,23 @@
   </si>
   <si>
     <t xml:space="preserve">2B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*) Wajib diisi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**) Wajib salah satu diisi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="167" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -530,32 +523,40 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -563,27 +564,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -595,7 +580,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -681,29 +666,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.34"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="2" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -711,106 +695,107 @@
       <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="3" t="n">
         <v>12345678</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="0" t="n">
+        <v>834234243</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="B8" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1234567812345680</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="0" t="n">
+        <v>812398123</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="B12" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1234567812345680</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" display="email@sekolah.id"/>
@@ -818,8 +803,8 @@
     <hyperlink ref="B14" r:id="rId3" display="admin@gmail.id"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -838,41 +823,41 @@
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="1.89"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>29</v>
+    <row r="1" s="2" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -891,46 +876,46 @@
       <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="16.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.33"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+    <row r="1" s="8" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="I1" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,28 +923,28 @@
         <v>1234567812345680</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>87771444141</v>
       </c>
-      <c r="E2" s="11" t="n">
+      <c r="E2" s="9" t="n">
         <v>34358</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>1234567812345680</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,28 +952,28 @@
         <v>1234567812345680</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>87771444141</v>
       </c>
-      <c r="E3" s="11" t="n">
+      <c r="E3" s="9" t="n">
         <v>34358</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>1234567812345680</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -996,34 +981,34 @@
         <v>1234567812345680</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>87771444141</v>
       </c>
-      <c r="E4" s="11" t="n">
+      <c r="E4" s="9" t="n">
         <v>34358</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>1234567812345680</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1036,68 +1021,67 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.64"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>10000000</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>10000000</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1112,71 +1096,71 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.66"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="8"/>
+    <row r="1" s="8" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>75000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>75000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>30000</v>
@@ -1184,13 +1168,13 @@
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>20000</v>
@@ -1198,8 +1182,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1214,11 +1198,11 @@
   </sheetPr>
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y3" activeCellId="0" sqref="Y3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.11"/>
@@ -1229,7 +1213,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="41.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="33.79"/>
@@ -1247,309 +1231,319 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="18.33"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+    <row r="1" s="8" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="D1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="M1" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="N1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="14" t="n">
+        <v>37948</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="13" t="n">
+        <v>715311312</v>
+      </c>
+      <c r="K2" s="13" t="n">
+        <v>117047387</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="13" t="n">
+        <v>706946036</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="R2" s="14"/>
+      <c r="S2" s="13" t="n">
+        <v>611875383</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="V2" s="14"/>
+      <c r="W2" s="13" t="n">
+        <v>987958880</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y2" s="13" t="n">
+        <v>50000</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="W1" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="X1" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z1" s="8" t="s">
+      <c r="D3" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" s="15" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E2" s="16" t="n">
-        <v>37948</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" s="15" t="n">
-        <v>715311312</v>
-      </c>
-      <c r="K2" s="15" t="n">
-        <v>117047387</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="O2" s="15" t="n">
-        <v>706946036</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="R2" s="16"/>
-      <c r="S2" s="15" t="n">
-        <v>611875383</v>
-      </c>
-      <c r="T2" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="U2" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="V2" s="16"/>
-      <c r="W2" s="15" t="n">
-        <v>987958880</v>
-      </c>
-      <c r="X2" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y2" s="15" t="n">
+      <c r="G3" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="13" t="n">
+        <v>533685358</v>
+      </c>
+      <c r="K3" s="13" t="n">
+        <v>983472148</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="O3" s="13" t="n">
+        <v>806298070</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="R3" s="14"/>
+      <c r="S3" s="13" t="n">
+        <v>133124861</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y3" s="13" t="n">
         <v>50000</v>
       </c>
-      <c r="Z2" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="Z3" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="J3" s="15" t="n">
-        <v>533685358</v>
-      </c>
-      <c r="K3" s="15" t="n">
-        <v>983472148</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="N3" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="O3" s="15" t="n">
-        <v>806298070</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q3" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="R3" s="16"/>
-      <c r="S3" s="15" t="n">
-        <v>133124861</v>
-      </c>
-      <c r="X3" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" s="15" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="15" t="s">
+      <c r="I4" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="15" t="s">
+      <c r="J4" s="13" t="n">
+        <v>130112285</v>
+      </c>
+      <c r="K4" s="13" t="n">
+        <v>396580957</v>
+      </c>
+      <c r="L4" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="M4" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" s="15" t="s">
+      <c r="N4" s="14"/>
+      <c r="O4" s="13" t="n">
+        <v>491574179</v>
+      </c>
+      <c r="P4" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="I4" s="15" t="s">
+      <c r="Q4" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="R4" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="J4" s="15" t="n">
-        <v>130112285</v>
-      </c>
-      <c r="K4" s="15" t="n">
-        <v>396580957</v>
-      </c>
-      <c r="L4" s="15" t="s">
+      <c r="S4" s="13" t="n">
+        <v>206641846</v>
+      </c>
+      <c r="T4" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="U4" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="N4" s="16"/>
-      <c r="O4" s="15" t="n">
-        <v>491574179</v>
-      </c>
-      <c r="P4" s="15" t="s">
+      <c r="V4" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="Q4" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="R4" s="15" t="s">
+      <c r="W4" s="13" t="n">
+        <v>482675675</v>
+      </c>
+      <c r="X4" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="S4" s="15" t="n">
-        <v>206641846</v>
-      </c>
-      <c r="T4" s="15" t="s">
+      <c r="Y4" s="13" t="n">
+        <v>50000</v>
+      </c>
+      <c r="Z4" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q7" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="U4" s="16" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15"/>
+      <c r="Q8" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="V4" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="W4" s="15" t="n">
-        <v>482675675</v>
-      </c>
-      <c r="X4" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y4" s="15" t="n">
-        <v>50000</v>
-      </c>
-      <c r="Z4" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q7" s="16"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17"/>
-      <c r="Q8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17"/>
+      <c r="A9" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1560,8 +1554,8 @@
     <hyperlink ref="V4" r:id="rId5" display="YulianaUsyiHalimah@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
chore: add all feature documentation (#15)
* chore: add all feature documentation

* fix: naming

* fix

* fix

---------

Co-authored-by: reynold <reynold@pop-os.localdomain>
</commit_message>
<xml_diff>
--- a/static/file/schools_import.xlsx
+++ b/static/file/schools_import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="122">
   <si>
     <t xml:space="preserve">Data Umum Sekolah</t>
   </si>
@@ -33,7 +33,7 @@
     <t xml:space="preserve">Nama Sekolah</t>
   </si>
   <si>
-    <t xml:space="preserve">SD Negeri 01 Pagi</t>
+    <t xml:space="preserve">nama sekolah</t>
   </si>
   <si>
     <t xml:space="preserve">Nomor Pokok Sekolah Nasional</t>
@@ -48,7 +48,7 @@
     <t xml:space="preserve">Alamat</t>
   </si>
   <si>
-    <t xml:space="preserve">Jalan Raya no 101 RT 003/004</t>
+    <t xml:space="preserve">alamat </t>
   </si>
   <si>
     <t xml:space="preserve">Email Sekolah (email resmi utk kontak)</t>
@@ -60,21 +60,15 @@
     <t xml:space="preserve">No Telpon Sekolah</t>
   </si>
   <si>
-    <t xml:space="preserve">081212341234</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nama Kepsek / Penanggungjawab Umum</t>
   </si>
   <si>
-    <t xml:space="preserve">Albert Einstein</t>
+    <t xml:space="preserve">kepsek</t>
   </si>
   <si>
     <t xml:space="preserve">NIK Kepsek</t>
   </si>
   <si>
-    <t xml:space="preserve">1234567812345678</t>
-  </si>
-  <si>
     <t xml:space="preserve">Email Kepsek</t>
   </si>
   <si>
@@ -84,21 +78,15 @@
     <t xml:space="preserve">No Telpon Kepsek (WA)</t>
   </si>
   <si>
-    <t xml:space="preserve">081343214321</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nama Admin (bila beda dgn Kepsek)</t>
   </si>
   <si>
-    <t xml:space="preserve">John Doe</t>
+    <t xml:space="preserve">admin</t>
   </si>
   <si>
     <t xml:space="preserve">NIK Admin</t>
   </si>
   <si>
-    <t xml:space="preserve">8765432187654321</t>
-  </si>
-  <si>
     <t xml:space="preserve">Email Admin</t>
   </si>
   <si>
@@ -397,18 +385,23 @@
   </si>
   <si>
     <t xml:space="preserve">2B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*) Wajib diisi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**) Wajib salah satu diisi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="167" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -530,32 +523,40 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -563,27 +564,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -595,7 +580,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -681,29 +666,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.34"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="2" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -711,106 +695,107 @@
       <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="3" t="n">
         <v>12345678</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="0" t="n">
+        <v>834234243</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="B8" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1234567812345680</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="0" t="n">
+        <v>812398123</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="B12" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1234567812345680</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" display="email@sekolah.id"/>
@@ -818,8 +803,8 @@
     <hyperlink ref="B14" r:id="rId3" display="admin@gmail.id"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -838,41 +823,41 @@
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="1.89"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>29</v>
+    <row r="1" s="2" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -891,46 +876,46 @@
       <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="16.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.33"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+    <row r="1" s="8" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="I1" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,28 +923,28 @@
         <v>1234567812345680</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>87771444141</v>
       </c>
-      <c r="E2" s="11" t="n">
+      <c r="E2" s="9" t="n">
         <v>34358</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>1234567812345680</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,28 +952,28 @@
         <v>1234567812345680</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>87771444141</v>
       </c>
-      <c r="E3" s="11" t="n">
+      <c r="E3" s="9" t="n">
         <v>34358</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>1234567812345680</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -996,34 +981,34 @@
         <v>1234567812345680</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>87771444141</v>
       </c>
-      <c r="E4" s="11" t="n">
+      <c r="E4" s="9" t="n">
         <v>34358</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>1234567812345680</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1036,68 +1021,67 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.64"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>10000000</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>10000000</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1112,71 +1096,71 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.66"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="8"/>
+    <row r="1" s="8" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>75000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>75000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>30000</v>
@@ -1184,13 +1168,13 @@
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>20000</v>
@@ -1198,8 +1182,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1214,11 +1198,11 @@
   </sheetPr>
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y3" activeCellId="0" sqref="Y3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.11"/>
@@ -1229,7 +1213,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="41.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="33.79"/>
@@ -1247,309 +1231,319 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="18.33"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+    <row r="1" s="8" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="D1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="M1" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="N1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="14" t="n">
+        <v>37948</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="13" t="n">
+        <v>715311312</v>
+      </c>
+      <c r="K2" s="13" t="n">
+        <v>117047387</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="13" t="n">
+        <v>706946036</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="R2" s="14"/>
+      <c r="S2" s="13" t="n">
+        <v>611875383</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="V2" s="14"/>
+      <c r="W2" s="13" t="n">
+        <v>987958880</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y2" s="13" t="n">
+        <v>50000</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="W1" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="X1" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z1" s="8" t="s">
+      <c r="D3" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" s="15" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E2" s="16" t="n">
-        <v>37948</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" s="15" t="n">
-        <v>715311312</v>
-      </c>
-      <c r="K2" s="15" t="n">
-        <v>117047387</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="O2" s="15" t="n">
-        <v>706946036</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="R2" s="16"/>
-      <c r="S2" s="15" t="n">
-        <v>611875383</v>
-      </c>
-      <c r="T2" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="U2" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="V2" s="16"/>
-      <c r="W2" s="15" t="n">
-        <v>987958880</v>
-      </c>
-      <c r="X2" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y2" s="15" t="n">
+      <c r="G3" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="13" t="n">
+        <v>533685358</v>
+      </c>
+      <c r="K3" s="13" t="n">
+        <v>983472148</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="O3" s="13" t="n">
+        <v>806298070</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="R3" s="14"/>
+      <c r="S3" s="13" t="n">
+        <v>133124861</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y3" s="13" t="n">
         <v>50000</v>
       </c>
-      <c r="Z2" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="Z3" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" s="13" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="J3" s="15" t="n">
-        <v>533685358</v>
-      </c>
-      <c r="K3" s="15" t="n">
-        <v>983472148</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="N3" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="O3" s="15" t="n">
-        <v>806298070</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q3" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="R3" s="16"/>
-      <c r="S3" s="15" t="n">
-        <v>133124861</v>
-      </c>
-      <c r="X3" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" s="15" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="15" t="s">
+      <c r="I4" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="15" t="s">
+      <c r="J4" s="13" t="n">
+        <v>130112285</v>
+      </c>
+      <c r="K4" s="13" t="n">
+        <v>396580957</v>
+      </c>
+      <c r="L4" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="M4" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" s="15" t="s">
+      <c r="N4" s="14"/>
+      <c r="O4" s="13" t="n">
+        <v>491574179</v>
+      </c>
+      <c r="P4" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="I4" s="15" t="s">
+      <c r="Q4" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="R4" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="J4" s="15" t="n">
-        <v>130112285</v>
-      </c>
-      <c r="K4" s="15" t="n">
-        <v>396580957</v>
-      </c>
-      <c r="L4" s="15" t="s">
+      <c r="S4" s="13" t="n">
+        <v>206641846</v>
+      </c>
+      <c r="T4" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="U4" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="N4" s="16"/>
-      <c r="O4" s="15" t="n">
-        <v>491574179</v>
-      </c>
-      <c r="P4" s="15" t="s">
+      <c r="V4" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="Q4" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="R4" s="15" t="s">
+      <c r="W4" s="13" t="n">
+        <v>482675675</v>
+      </c>
+      <c r="X4" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="S4" s="15" t="n">
-        <v>206641846</v>
-      </c>
-      <c r="T4" s="15" t="s">
+      <c r="Y4" s="13" t="n">
+        <v>50000</v>
+      </c>
+      <c r="Z4" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q7" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="U4" s="16" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15"/>
+      <c r="Q8" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="V4" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="W4" s="15" t="n">
-        <v>482675675</v>
-      </c>
-      <c r="X4" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y4" s="15" t="n">
-        <v>50000</v>
-      </c>
-      <c r="Z4" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q7" s="16"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17"/>
-      <c r="Q8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17"/>
+      <c r="A9" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1560,8 +1554,8 @@
     <hyperlink ref="V4" r:id="rId5" display="YulianaUsyiHalimah@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>